<commit_message>
mass  & moments of inertia
</commit_message>
<xml_diff>
--- a/Technical/Technical Budgets/PowerMassBOM_ABee_NEW.xlsx
+++ b/Technical/Technical Budgets/PowerMassBOM_ABee_NEW.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="13680" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Battery" sheetId="1" r:id="rId1"/>
@@ -37,27 +37,27 @@
     <definedName name="ElecTypCur">Electronics!$L$15</definedName>
     <definedName name="ElecTypPow">Electronics!$F$15</definedName>
     <definedName name="ElecTypVolt">Electronics!$I$15</definedName>
-    <definedName name="PropCost">Propulsion!$D$5</definedName>
-    <definedName name="PropMass">Propulsion!$C$5</definedName>
-    <definedName name="PropMaxCur">Propulsion!$O$5</definedName>
-    <definedName name="PropMaxPow">Propulsion!$I$5</definedName>
-    <definedName name="PropMaxVolt">Propulsion!$L$5</definedName>
-    <definedName name="PropMinCur">Propulsion!$M$5</definedName>
-    <definedName name="PropMinPow">Propulsion!$G$5</definedName>
-    <definedName name="PropMinVolt">Propulsion!$J$5</definedName>
-    <definedName name="PropQty">Propulsion!$B$5</definedName>
-    <definedName name="PropThrustMax">Propulsion!$F$5</definedName>
-    <definedName name="PropThrustNom">Propulsion!$E$5</definedName>
-    <definedName name="PropTypCur">Propulsion!$N$5</definedName>
-    <definedName name="PropTypPow">Propulsion!$H$5</definedName>
-    <definedName name="PropTypVolt">Propulsion!$K$5</definedName>
+    <definedName name="PropCost">Propulsion!$D$6</definedName>
+    <definedName name="PropMass">Propulsion!$C$6</definedName>
+    <definedName name="PropMaxCur">Propulsion!$O$6</definedName>
+    <definedName name="PropMaxPow">Propulsion!$I$6</definedName>
+    <definedName name="PropMaxVolt">Propulsion!$L$6</definedName>
+    <definedName name="PropMinCur">Propulsion!$M$6</definedName>
+    <definedName name="PropMinPow">Propulsion!$G$6</definedName>
+    <definedName name="PropMinVolt">Propulsion!$J$6</definedName>
+    <definedName name="PropQty">Propulsion!$B$6</definedName>
+    <definedName name="PropThrustMax">Propulsion!$F$6</definedName>
+    <definedName name="PropThrustNom">Propulsion!$E$6</definedName>
+    <definedName name="PropTypCur">Propulsion!$N$6</definedName>
+    <definedName name="PropTypPow">Propulsion!$H$6</definedName>
+    <definedName name="PropTypVolt">Propulsion!$K$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
   <si>
     <t>Battery</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>FrSky TFR4 Radio Reciever</t>
+  </si>
+  <si>
+    <t>20 A ESC</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -884,6 +887,7 @@
     <xf numFmtId="11" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -947,7 +951,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1252,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,72 +1270,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="113" t="s">
+      <c r="E2" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="117" t="s">
+      <c r="G2" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="115" t="s">
+      <c r="H2" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="119" t="s">
+      <c r="I2" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="119" t="s">
+      <c r="J2" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="119" t="s">
+      <c r="K2" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="107" t="s">
+      <c r="L2" s="108" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="108"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="109"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
@@ -1369,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="51">
-        <f t="shared" si="0"/>
+        <f>B4*C4</f>
         <v>815.8</v>
       </c>
       <c r="D5" s="52">
@@ -1468,7 +1474,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1480,60 +1486,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="121" t="s">
+      <c r="E2" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="121" t="s">
+      <c r="F2" s="123"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="122"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="121" t="s">
+      <c r="I2" s="123"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="122"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="107" t="s">
+      <c r="L2" s="123"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="108" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="112"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="113"/>
       <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
@@ -1561,7 +1567,7 @@
       <c r="M3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="108"/>
+      <c r="N3" s="109"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
@@ -1606,7 +1612,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="100" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="127" t="s">
+      <c r="A5" s="106" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="97">
@@ -1656,7 +1662,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="100" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="127" t="s">
+      <c r="A7" s="106" t="s">
         <v>81</v>
       </c>
       <c r="B7" s="97">
@@ -1926,7 +1932,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="45">
-        <f>B4*C4+B6*C6+B8*C8+B9*C9+B10*C10+B11*C11+B12*C12+B13*C13+B14*C14</f>
+        <f>B4*C4+B6*C6+B8*C8+B9*C9+B10*C10+B11*C11+B12*C12+B13*C13+B14*C14+B5*C5+B7*C7</f>
         <v>586.54999999999995</v>
       </c>
       <c r="D15" s="46">
@@ -2019,7 +2025,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2030,52 +2036,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="119" t="s">
+      <c r="E2" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="119" t="s">
+      <c r="F2" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="119" t="s">
+      <c r="G2" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="107" t="s">
+      <c r="H2" s="108" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="108"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="109"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
@@ -2134,7 +2140,7 @@
         <v>43</v>
       </c>
       <c r="B7" s="73">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="73">
         <v>39</v>
@@ -2169,11 +2175,11 @@
       </c>
       <c r="B9" s="24">
         <f>SUM(B4:B8)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="48">
         <f>C8*B8+B7*C7+C5*B5+B4*C4+C6*B6</f>
-        <v>549</v>
+        <v>471</v>
       </c>
       <c r="D9" s="49">
         <f>SUM(D4:D8)</f>
@@ -2211,18 +2217,15 @@
     <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="C9" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2233,46 +2236,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="111" t="s">
+      <c r="D1" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="121" t="s">
+      <c r="E1" s="122" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="123"/>
-      <c r="G1" s="121" t="s">
+      <c r="F1" s="124"/>
+      <c r="G1" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="122"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="121" t="s">
+      <c r="H1" s="123"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="122"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="121" t="s">
+      <c r="K1" s="123"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="122"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="107" t="s">
+      <c r="N1" s="123"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="108" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="110"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="112"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="113"/>
       <c r="E2" s="26" t="s">
         <v>28</v>
       </c>
@@ -2306,7 +2309,7 @@
       <c r="O2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="108"/>
+      <c r="P2" s="109"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -2316,8 +2319,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="63">
-        <f>65+28.4</f>
-        <v>93.4</v>
+        <v>68.7</v>
       </c>
       <c r="D3" s="64"/>
       <c r="E3" s="67"/>
@@ -2334,8 +2336,8 @@
       <c r="L3" s="71"/>
       <c r="M3" s="69"/>
       <c r="N3" s="105">
-        <f>N8*(TOTAL!C8/4)*(TOTAL!C8/4)+Propulsion!N9*(TOTAL!C8/4)+Propulsion!N10</f>
-        <v>4.7453291022096877</v>
+        <f>N9*(TOTAL!C8/4)*(TOTAL!C8/4)+Propulsion!N10*(TOTAL!C8/4)+Propulsion!N11</f>
+        <v>4.5238328166596862</v>
       </c>
       <c r="O3" s="71">
         <v>20000</v>
@@ -2344,165 +2346,189 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="100" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B4" s="41">
         <v>4</v>
       </c>
       <c r="C4" s="41">
-        <v>11.1</v>
+        <v>28.4</v>
       </c>
       <c r="D4" s="42"/>
       <c r="E4" s="44"/>
       <c r="F4" s="43"/>
       <c r="G4" s="58"/>
-      <c r="H4" s="59"/>
+      <c r="H4" s="128"/>
       <c r="I4" s="60"/>
       <c r="J4" s="59"/>
       <c r="K4" s="59"/>
       <c r="L4" s="60"/>
       <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
+      <c r="N4" s="128"/>
       <c r="O4" s="60"/>
       <c r="P4" s="39"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:16" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="41">
+        <v>4</v>
+      </c>
+      <c r="C5" s="41">
+        <v>11.1</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="39"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="29">
-        <f t="shared" ref="B5:M5" si="0">SUM(B3:B4)</f>
-        <v>8</v>
-      </c>
-      <c r="C5" s="47">
-        <f>B4*C4+B3*C3</f>
-        <v>418</v>
-      </c>
-      <c r="D5" s="47">
+      <c r="B6" s="29">
+        <f t="shared" ref="B6:M6" si="0">SUM(B3:B5)</f>
+        <v>12</v>
+      </c>
+      <c r="C6" s="47">
+        <f>B5*C5+B3*C3+B4*C4</f>
+        <v>432.79999999999995</v>
+      </c>
+      <c r="D6" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E6" s="47">
         <f>4*E3</f>
         <v>0</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F6" s="47">
         <f>4*F3:F3</f>
         <v>4800</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G6" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H6" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I6" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J6" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K6" s="47">
         <f t="shared" si="0"/>
         <v>14.8</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L6" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M6" s="47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N6" s="47">
         <f>4*N3*1000</f>
-        <v>18981.316408838749</v>
-      </c>
-      <c r="O5" s="47">
+        <v>18095.331266638746</v>
+      </c>
+      <c r="O6" s="47">
         <f>4*O3</f>
         <v>80000</v>
       </c>
-      <c r="P5" s="30"/>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="57"/>
-      <c r="H6" s="57">
+      <c r="P6" s="30"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="57"/>
+      <c r="H7" s="57">
         <f>PropTypVolt*PropTypCur</f>
-        <v>280923.48285081348</v>
-      </c>
-      <c r="I6" s="57">
+        <v>267810.90274625347</v>
+      </c>
+      <c r="I7" s="57">
         <f>PropMaxCur*PropTypVolt</f>
         <v>1184000</v>
       </c>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="61"/>
-      <c r="O6" s="61"/>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55" t="s">
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="N7" s="56" t="s">
+      <c r="N8" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="O7" s="62" t="s">
+      <c r="O8" s="62" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" t="s">
-        <v>74</v>
-      </c>
-      <c r="N8" s="104">
-        <v>4.7180000000000004E-6</v>
-      </c>
-      <c r="O8" s="54"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G9" s="56"/>
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
       <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
       <c r="L9" s="56"/>
       <c r="M9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" s="104">
+        <v>4.7180000000000004E-6</v>
+      </c>
+      <c r="O9" s="54"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="54">
+      <c r="N10" s="54">
         <v>8.5039999999999994E-3</v>
       </c>
-      <c r="O9" s="54"/>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M10" t="s">
+      <c r="O10" s="54"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
         <v>76</v>
       </c>
-      <c r="N10">
+      <c r="N11">
         <v>-1.947284</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2526,8 +2552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,22 +2564,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="109"/>
-      <c r="B2" s="107" t="s">
+      <c r="A2" s="110"/>
+      <c r="B2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="112" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="112"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="113"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2578,11 +2604,11 @@
       </c>
       <c r="B5" s="5">
         <f>PropQty</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5">
         <f>PropMass</f>
-        <v>418</v>
+        <v>432.79999999999995</v>
       </c>
       <c r="D5" s="6">
         <f>PropCost</f>
@@ -2595,41 +2621,41 @@
       </c>
       <c r="B6" s="8">
         <f>DeadMassQty</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="8">
         <f>DeadMass</f>
-        <v>549</v>
+        <v>471</v>
       </c>
       <c r="D6" s="9">
         <f>PropMass</f>
-        <v>418</v>
-      </c>
-      <c r="E6" s="124" t="s">
+        <v>432.79999999999995</v>
+      </c>
+      <c r="E6" s="125" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="125" t="s">
+      <c r="F6" s="126" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="124" t="s">
+      <c r="G6" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="125" t="s">
+      <c r="H6" s="126" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="124" t="s">
+      <c r="I6" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="124" t="s">
+      <c r="J6" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="124" t="s">
+      <c r="K6" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="124" t="s">
+      <c r="L6" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="124" t="s">
+      <c r="M6" s="125" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2649,15 +2675,15 @@
         <f>BattCostTot</f>
         <v>0</v>
       </c>
-      <c r="E7" s="124"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="124"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="125"/>
     </row>
     <row r="8" spans="1:13" s="85" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
@@ -2665,15 +2691,15 @@
       </c>
       <c r="B8" s="83">
         <f>B4+B5+B6+B7</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="83">
         <f>C4+C5+C6+C7</f>
-        <v>2369.35</v>
+        <v>2306.1499999999996</v>
       </c>
       <c r="D8" s="84">
         <f t="shared" ref="D8" si="0">D4+D5+D6+D7</f>
-        <v>1004.55</v>
+        <v>1019.3499999999999</v>
       </c>
       <c r="E8" s="101">
         <f>PropThrustNom</f>
@@ -2685,7 +2711,7 @@
       </c>
       <c r="G8" s="101">
         <f>2*C8</f>
-        <v>4738.7</v>
+        <v>4612.2999999999993</v>
       </c>
       <c r="H8" s="101">
         <f>BattCap</f>
@@ -2701,11 +2727,11 @@
       </c>
       <c r="K8" s="102">
         <f>ElecTypCur+PropTypCur</f>
-        <v>24145.69864822099</v>
+        <v>23259.713506020984</v>
       </c>
       <c r="L8" s="101">
         <f>(H8/1000)/((K8/1000))*60</f>
-        <v>24.84914637349733</v>
+        <v>25.795674561713096</v>
       </c>
       <c r="M8" s="101">
         <f>(H8/1000)/(J8/1000)*60</f>
@@ -2718,7 +2744,7 @@
       </c>
       <c r="G9">
         <f>G8/4</f>
-        <v>1184.675</v>
+        <v>1153.0749999999998</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2727,7 +2753,7 @@
       </c>
       <c r="G10">
         <f>G9/2</f>
-        <v>592.33749999999998</v>
+        <v>576.53749999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a whole bunch of good stuffz
</commit_message>
<xml_diff>
--- a/Technical/Technical Budgets/PowerMassBOM_ABee_NEW.xlsx
+++ b/Technical/Technical Budgets/PowerMassBOM_ABee_NEW.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="13680"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="24240" windowHeight="13680" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Battery" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
   <si>
     <t>Battery</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>20 A ESC</t>
+  </si>
+  <si>
+    <t>*80% of total used</t>
   </si>
 </sst>
 </file>
@@ -888,6 +891,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -950,9 +956,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1258,7 +1261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1270,72 +1273,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="114" t="s">
+      <c r="E2" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="116" t="s">
+      <c r="F2" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="118" t="s">
+      <c r="G2" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="116" t="s">
+      <c r="H2" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="120" t="s">
+      <c r="I2" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="120" t="s">
+      <c r="J2" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="120" t="s">
+      <c r="K2" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="108" t="s">
+      <c r="L2" s="109" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="109"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="110"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
@@ -1486,60 +1489,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="122" t="s">
+      <c r="E2" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="123"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="122" t="s">
+      <c r="F2" s="124"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="123"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="122" t="s">
+      <c r="I2" s="124"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="123"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="108" t="s">
+      <c r="L2" s="124"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="109" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="113"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="114"/>
       <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1570,7 @@
       <c r="M3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="109"/>
+      <c r="N3" s="110"/>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
@@ -2036,52 +2039,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="120" t="s">
+      <c r="E2" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="120" t="s">
+      <c r="F2" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="120" t="s">
+      <c r="G2" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="109" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="109"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="110"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
@@ -2224,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2236,46 +2239,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="122" t="s">
+      <c r="E1" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="124"/>
-      <c r="G1" s="122" t="s">
+      <c r="F1" s="125"/>
+      <c r="G1" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="123"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="122" t="s">
+      <c r="H1" s="124"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="123"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="122" t="s">
+      <c r="K1" s="124"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="123"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="108" t="s">
+      <c r="N1" s="124"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="109" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="113"/>
+      <c r="A2" s="112"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="114"/>
       <c r="E2" s="26" t="s">
         <v>28</v>
       </c>
@@ -2309,7 +2312,7 @@
       <c r="O2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="109"/>
+      <c r="P2" s="110"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -2360,13 +2363,13 @@
       <c r="E4" s="44"/>
       <c r="F4" s="43"/>
       <c r="G4" s="58"/>
-      <c r="H4" s="128"/>
+      <c r="H4" s="107"/>
       <c r="I4" s="60"/>
       <c r="J4" s="59"/>
       <c r="K4" s="59"/>
       <c r="L4" s="60"/>
       <c r="M4" s="59"/>
-      <c r="N4" s="128"/>
+      <c r="N4" s="107"/>
       <c r="O4" s="60"/>
       <c r="P4" s="39"/>
     </row>
@@ -2552,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,22 +2567,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="110"/>
-      <c r="B2" s="108" t="s">
+      <c r="A2" s="111"/>
+      <c r="B2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="113" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="113"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="114"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2631,31 +2634,31 @@
         <f>PropMass</f>
         <v>432.79999999999995</v>
       </c>
-      <c r="E6" s="125" t="s">
+      <c r="E6" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="126" t="s">
+      <c r="F6" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="125" t="s">
+      <c r="G6" s="126" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="126" t="s">
+      <c r="H6" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="125" t="s">
+      <c r="I6" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="125" t="s">
+      <c r="J6" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="125" t="s">
+      <c r="K6" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="125" t="s">
+      <c r="L6" s="126" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="125" t="s">
+      <c r="M6" s="126" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2675,15 +2678,15 @@
         <f>BattCostTot</f>
         <v>0</v>
       </c>
-      <c r="E7" s="125"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="125"/>
-      <c r="J7" s="125"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="125"/>
-      <c r="M7" s="125"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="126"/>
     </row>
     <row r="8" spans="1:13" s="85" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
@@ -2714,8 +2717,8 @@
         <v>4612.2999999999993</v>
       </c>
       <c r="H8" s="101">
-        <f>BattCap</f>
-        <v>10000</v>
+        <f>BattCap*0.8</f>
+        <v>8000</v>
       </c>
       <c r="I8" s="101">
         <f>ElecTypPow+PropTypPow</f>
@@ -2731,11 +2734,11 @@
       </c>
       <c r="L8" s="101">
         <f>(H8/1000)/((K8/1000))*60</f>
-        <v>25.795674561713096</v>
+        <v>20.636539649370476</v>
       </c>
       <c r="M8" s="101">
         <f>(H8/1000)/(J8/1000)*60</f>
-        <v>7.0451987582497173</v>
+        <v>5.6361590065997742</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2745,6 +2748,9 @@
       <c r="G9">
         <f>G8/4</f>
         <v>1153.0749999999998</v>
+      </c>
+      <c r="H9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>